<commit_message>
Working part 1 of assingment 8
Yet to optimize and do unknown characteristic part
</commit_message>
<xml_diff>
--- a/questions/Assignment 7 - Blue Gecko Command Table.xlsx
+++ b/questions/Assignment 7 - Blue Gecko Command Table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohit\SimplicityStudio\v4_workspace\ecen5823-assignments\questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB1D407-96BB-49CE-AE66-7E3FBAB233F1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F07F6DB-FBDB-4C13-907A-00103289FC73}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -377,7 +377,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -452,6 +452,12 @@
       <color theme="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -493,7 +499,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -530,6 +536,9 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -852,7 +861,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16:XFD16"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1961,7 +1970,7 @@
       <c r="A26" s="12"/>
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A27" s="12"/>
+      <c r="A27" s="20"/>
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1">
       <c r="A28" s="12"/>
@@ -4845,5 +4854,6 @@
     <hyperlink ref="E11" r:id="rId25" location="cmd_gatt_set_characteristic_notification" xr:uid="{E11EC0C2-1802-4031-B3BC-6B9D0B030616}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>